<commit_message>
Add benchmarking discussion to README.md
</commit_message>
<xml_diff>
--- a/test/sizes.xlsx
+++ b/test/sizes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameszhang/Documents/Cornell/Courses/Senior Spring/ORIE 4742/Project/Arithmetic-Coding/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F1050D-5945-2440-8EBB-D2ED6DC63B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA49409B-F42C-964E-87A5-A8CF8923C639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="1840" windowWidth="28040" windowHeight="17420" xr2:uid="{D32BA931-7593-024E-BAAE-B922191094BC}"/>
+    <workbookView xWindow="440" yWindow="1320" windowWidth="28040" windowHeight="17420" xr2:uid="{D32BA931-7593-024E-BAAE-B922191094BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
   <si>
     <t>alice_full</t>
   </si>
@@ -459,9 +459,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77111E0D-43C3-6C4E-BB7B-9B9312D71C4A}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="144" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1109,7 +1111,330 @@
         <v>0.87696499999999999</v>
       </c>
     </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1">
+        <f t="shared" ref="B26:H26" si="10">B3/B$2</f>
+        <v>0.43387052151058236</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="10"/>
+        <v>9.0000000000000002E-6</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="10"/>
+        <v>0.56534300000000004</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="10"/>
+        <v>1.8880000000000001E-2</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="10"/>
+        <v>0.41596489147194876</v>
+      </c>
+      <c r="G26" s="1">
+        <f t="shared" si="10"/>
+        <v>0.12501499999999999</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="10"/>
+        <v>0.87358100000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" ref="B27:H27" si="11">B4/B$2</f>
+        <v>0.44874118135288421</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="11"/>
+        <v>2.32E-4</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="11"/>
+        <v>0.55715400000000004</v>
+      </c>
+      <c r="E27" s="1">
+        <f t="shared" si="11"/>
+        <v>2.1624999999999998E-2</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="11"/>
+        <v>0.43221444668485354</v>
+      </c>
+      <c r="G27" s="1">
+        <f t="shared" si="11"/>
+        <v>0.12542800000000001</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="11"/>
+        <v>0.86348999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" ref="B28:H28" si="12">B5/B$2</f>
+        <v>0.6591160603126297</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="12"/>
+        <v>1.2281E-2</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="12"/>
+        <v>0.62212100000000004</v>
+      </c>
+      <c r="E28" s="1">
+        <f t="shared" si="12"/>
+        <v>3.5964000000000003E-2</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="12"/>
+        <v>0.64389356739018699</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" si="12"/>
+        <v>0.146097</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="12"/>
+        <v>0.86191200000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" ref="B29:H29" si="13">B6/B$2</f>
+        <v>0.54868584866509895</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="13"/>
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="13"/>
+        <v>0.552319</v>
+      </c>
+      <c r="E29" s="1">
+        <f t="shared" si="13"/>
+        <v>1.8676000000000002E-2</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="13"/>
+        <v>0.45688530423437312</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="13"/>
+        <v>0.12500900000000001</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="13"/>
+        <v>0.85869200000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" ref="B30:H30" si="14">B7/B$2</f>
+        <v>0.5490593443076498</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="14"/>
+        <v>2.32E-4</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="14"/>
+        <v>0.55225500000000005</v>
+      </c>
+      <c r="E30" s="1">
+        <f t="shared" si="14"/>
+        <v>1.8699E-2</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="14"/>
+        <v>0.45833498069294537</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="14"/>
+        <v>0.12523000000000001</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="14"/>
+        <v>0.85861299999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" ref="B31:H31" si="15">B8/B$2</f>
+        <v>0.58096555540185368</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="15"/>
+        <v>1.2279999999999999E-2</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="15"/>
+        <v>0.553894</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="15"/>
+        <v>2.8063999999999999E-2</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="15"/>
+        <v>0.516519722189275</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="15"/>
+        <v>0.13712199999999999</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="15"/>
+        <v>0.85879000000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1">
+        <f>B10/B$2</f>
+        <v>0.55255222022409733</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" ref="C32:H33" si="16">C10/C$2</f>
+        <v>0.125001</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="16"/>
+        <v>0.55318699999999998</v>
+      </c>
+      <c r="E32" s="1">
+        <f t="shared" si="16"/>
+        <v>0.133572</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="16"/>
+        <v>0.4603645277349464</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="16"/>
+        <v>0.18741099999999999</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="16"/>
+        <v>0.86024800000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="1">
+        <f>B11/B$2</f>
+        <v>0.36536173744639644</v>
+      </c>
+      <c r="C33" s="1">
+        <f t="shared" si="16"/>
+        <v>1.1540000000000001E-3</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="16"/>
+        <v>0.65231899999999998</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="16"/>
+        <v>3.3461999999999999E-2</v>
+      </c>
+      <c r="F33" s="1">
+        <f t="shared" si="16"/>
+        <v>0.3689294798297289</v>
+      </c>
+      <c r="G33" s="1">
+        <f t="shared" si="16"/>
+        <v>0.15914400000000001</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="16"/>
+        <v>0.87696499999999999</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B14:B23">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:H23">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:H33">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>